<commit_message>
evaluations and finish with gravity
</commit_message>
<xml_diff>
--- a/Smart_Nodes_Routing/Evaluations.xlsx
+++ b/Smart_Nodes_Routing/Evaluations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\PycharmProjects\Research_Implementing\Smart_Nodes_Routing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC4928E-DEB9-4D0F-9A9C-5924033701A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587D3F74-25F8-4379-9AA0-10DFBA25B37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="5" xr2:uid="{B550FEBA-CBDF-4F8A-ACA3-FAF0BB6C78BC}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" firstSheet="3" activeTab="5" xr2:uid="{B550FEBA-CBDF-4F8A-ACA3-FAF0BB6C78BC}"/>
   </bookViews>
   <sheets>
     <sheet name="China_Telecom_1024LP" sheetId="4" r:id="rId1"/>
@@ -334,12 +334,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -357,17 +366,8 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -532,7 +532,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.43875957990349113</c:v>
+                  <c:v>0.44195288106727215</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.2448197558898666</c:v>
@@ -622,7 +622,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.43124468386730941</c:v>
+                  <c:v>0.43606464417351831</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.25347320669123885</c:v>
@@ -712,7 +712,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.44604214123006836</c:v>
+                  <c:v>0.44397779043280194</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.25911161731207288</c:v>
@@ -773,7 +773,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.44110722693871729</c:v>
+                  <c:v>0.43846757508739409</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.25290718413355218</c:v>
@@ -1255,7 +1255,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.57571487287886791</c:v>
+                  <c:v>0.58017732370383412</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.13727907932593508</c:v>
@@ -1342,7 +1342,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.62043199065966115</c:v>
+                  <c:v>0.59427904261529463</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.13712784588441318</c:v>
@@ -1429,7 +1429,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.56777408209701097</c:v>
+                  <c:v>0.56343625139687337</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.14190462214431743</c:v>
@@ -1487,7 +1487,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.5706860706860708</c:v>
+                  <c:v>0.55122430122430122</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.13178563178563185</c:v>
@@ -1966,7 +1966,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.57571487287886791</c:v>
+                  <c:v>0.58017732370383412</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.13727907932593508</c:v>
@@ -2053,7 +2053,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.62043199065966115</c:v>
+                  <c:v>0.59427904261529463</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.13712784588441318</c:v>
@@ -2140,7 +2140,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.56777408209701097</c:v>
+                  <c:v>0.56343625139687337</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.14190462214431743</c:v>
@@ -2198,7 +2198,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.57443327880345874</c:v>
+                  <c:v>0.56935031549427451</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.14086235101659272</c:v>
@@ -2677,7 +2677,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.25221238938053103</c:v>
+                  <c:v>0.24610924626182484</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.15372291730241083</c:v>
@@ -2764,7 +2764,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.23252626770214713</c:v>
+                  <c:v>0.23359220344144993</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.15676869194457144</c:v>
@@ -2851,7 +2851,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.24523410096080545</c:v>
+                  <c:v>0.2425651974988563</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.15197498856184244</c:v>
@@ -2909,7 +2909,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.23090264685921125</c:v>
+                  <c:v>0.23746323806651071</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.13852650629665941</c:v>
@@ -3389,7 +3389,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.18650000000000011</c:v>
+                  <c:v>0.17959999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.12840000000000007</c:v>
@@ -3479,7 +3479,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.1745000000000001</c:v>
+                  <c:v>0.1754</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.12890000000000001</c:v>
@@ -3569,7 +3569,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.18149999999999999</c:v>
+                  <c:v>0.18300000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.12490000000000001</c:v>
@@ -3630,7 +3630,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.18389999999999995</c:v>
+                  <c:v>0.18870000000000009</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.125</c:v>
@@ -8855,8 +8855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0718E9FF-6293-4A98-AAC0-CA1B55B1C195}">
   <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8890,25 +8890,25 @@
         <v>2</v>
       </c>
       <c r="I1" s="3"/>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="8" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="8" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="8" t="s">
+      <c r="Q1" s="19"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="10"/>
+      <c r="T1" s="11"/>
       <c r="U1" s="3" t="s">
         <v>7</v>
       </c>
@@ -8926,25 +8926,25 @@
       <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="8" t="s">
+      <c r="N2" s="19"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="8" t="s">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="10"/>
+      <c r="T2" s="11"/>
       <c r="U2" s="3" t="s">
         <v>6</v>
       </c>
@@ -8953,25 +8953,25 @@
       <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="14">
         <v>1.4016999999999999</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="11">
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="14">
         <v>1.4092</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="11">
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="14">
         <v>1.4108000000000001</v>
       </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="14">
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="17">
         <v>1.4048</v>
       </c>
-      <c r="T3" s="15"/>
+      <c r="T3" s="18"/>
       <c r="U3" s="5">
         <v>1.4016999999999999</v>
       </c>
@@ -8983,23 +8983,23 @@
       <c r="J4" s="3">
         <v>6.8305999999999996</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="12">
         <f>ROUND(J4/J3,4)-1</f>
         <v>3.8731</v>
       </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="8">
+      <c r="L4" s="13"/>
+      <c r="M4" s="10">
         <v>7.6843000000000004</v>
       </c>
-      <c r="N4" s="10"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="6">
         <f>ROUND(M4/M3,4)-1</f>
         <v>4.4530000000000003</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="10">
         <v>7.6825999999999999</v>
       </c>
-      <c r="Q4" s="10"/>
+      <c r="Q4" s="11"/>
       <c r="R4" s="6">
         <f>ROUND(P4/P3,4)-1</f>
         <v>4.4455999999999998</v>
@@ -9019,23 +9019,23 @@
       <c r="J5" s="3">
         <v>2.1465000000000001</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="12">
         <f>ROUND(J5/J3,4)-1</f>
         <v>0.53140000000000009</v>
       </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="8">
+      <c r="L5" s="13"/>
+      <c r="M5" s="10">
         <v>2.1532</v>
       </c>
-      <c r="N5" s="10"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="6">
         <f>ROUND(M5/M3,4)-1</f>
         <v>0.52800000000000002</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="10">
         <v>2.1534</v>
       </c>
-      <c r="Q5" s="10"/>
+      <c r="Q5" s="11"/>
       <c r="R5" s="6">
         <f>ROUND(P5/P3,4)-1</f>
         <v>0.52639999999999998</v>
@@ -9055,23 +9055,23 @@
       <c r="J6" s="3">
         <v>2.29</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="12">
         <f>ROUND(J6/J3,4)-1</f>
         <v>0.63369999999999993</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="8">
+      <c r="L6" s="13"/>
+      <c r="M6" s="10">
         <v>2.2345000000000002</v>
       </c>
-      <c r="N6" s="10"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="6">
         <f>ROUND(M6/M3,4)-1</f>
         <v>0.58570000000000011</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="10">
         <v>2.23</v>
       </c>
-      <c r="Q6" s="10"/>
+      <c r="Q6" s="11"/>
       <c r="R6" s="6">
         <f>ROUND(P6/P3,4)-1</f>
         <v>0.58069999999999999</v>
@@ -9091,22 +9091,22 @@
       <c r="J11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="18" t="s">
+      <c r="L11" s="9"/>
+      <c r="M11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="8" t="s">
+      <c r="N11" s="9"/>
+      <c r="O11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="8" t="s">
+      <c r="P11" s="11"/>
+      <c r="Q11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="10"/>
+      <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="I12" s="2" t="s">
@@ -9116,32 +9116,32 @@
         <v>15</v>
       </c>
       <c r="K12" s="2">
-        <v>2.0274999999999999</v>
+        <v>2.032</v>
       </c>
       <c r="L12" s="6">
         <f>K12/M3-1</f>
-        <v>0.43875957990349113</v>
+        <v>0.44195288106727215</v>
       </c>
       <c r="M12" s="2">
-        <v>2.0192000000000001</v>
+        <v>2.0259999999999998</v>
       </c>
       <c r="N12" s="6">
         <f>M12/P3-1</f>
-        <v>0.43124468386730941</v>
+        <v>0.43606464417351831</v>
       </c>
       <c r="O12" s="3">
-        <v>2.0314000000000001</v>
+        <v>2.0285000000000002</v>
       </c>
       <c r="P12" s="6">
         <f>O12/S3-1</f>
-        <v>0.44604214123006836</v>
+        <v>0.44397779043280194</v>
       </c>
       <c r="Q12" s="3">
-        <v>2.02</v>
+        <v>2.0163000000000002</v>
       </c>
       <c r="R12" s="6">
         <f>Q12/U3-1</f>
-        <v>0.44110722693871729</v>
+        <v>0.43846757508739409</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -9358,6 +9358,1020 @@
       <c r="R18" s="6">
         <f>Q18/U3-1</f>
         <v>8.318470428765079E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="Q11:R11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDA6A5E-47CB-4971-B4D4-80E7225292CB}">
+  <dimension ref="A1:U17"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" customWidth="1"/>
+    <col min="19" max="19" width="22" customWidth="1"/>
+    <col min="20" max="20" width="24.5703125" customWidth="1"/>
+    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="19"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="11"/>
+      <c r="U1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>104</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="19"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="11"/>
+      <c r="U2" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="14">
+        <v>1.7073</v>
+      </c>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="14">
+        <v>1.7031000000000001</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="14">
+        <v>1.7130000000000001</v>
+      </c>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="17">
+        <v>1.7059218101262801</v>
+      </c>
+      <c r="T3" s="18"/>
+      <c r="U3" s="5">
+        <v>1.7316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3">
+        <v>136.69470000000001</v>
+      </c>
+      <c r="K4" s="20">
+        <f>ROUND(J4/J3,4)-1</f>
+        <v>79.064800000000005</v>
+      </c>
+      <c r="L4" s="21"/>
+      <c r="M4" s="10">
+        <v>132.49350000000001</v>
+      </c>
+      <c r="N4" s="11"/>
+      <c r="O4" s="7">
+        <f>ROUND(M4/M3,4)-1</f>
+        <v>76.795500000000004</v>
+      </c>
+      <c r="P4" s="10">
+        <v>151.20259999999999</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="6">
+        <f>ROUND(P4/P3,4)-1</f>
+        <v>87.267700000000005</v>
+      </c>
+      <c r="S4" s="3">
+        <v>49.514683496694197</v>
+      </c>
+      <c r="T4" s="7">
+        <f>ROUND(S4/S3,4)-1</f>
+        <v>28.025200000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2.5396999999999998</v>
+      </c>
+      <c r="K5" s="20">
+        <f>ROUND(J5/J3,4)-1</f>
+        <v>0.48760000000000003</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="10">
+        <v>2.5322</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5" s="7">
+        <f>ROUND(M5/M3,4)-1</f>
+        <v>0.4867999999999999</v>
+      </c>
+      <c r="P5" s="10">
+        <v>2.5428999999999999</v>
+      </c>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="6">
+        <f>ROUND(P5/P3,4)-1</f>
+        <v>0.48449999999999993</v>
+      </c>
+      <c r="S5" s="3">
+        <v>2.5407999999999999</v>
+      </c>
+      <c r="T5" s="7">
+        <f>ROUND(S5/S3,4)-1</f>
+        <v>0.48940000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2.5535000000000001</v>
+      </c>
+      <c r="K6" s="20">
+        <f>ROUND(J6/J3,4)-1</f>
+        <v>0.49560000000000004</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="10">
+        <v>2.9327999999999999</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="7">
+        <f>ROUND(M6/M3,4)-1</f>
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="P6" s="10">
+        <v>2.9142999999999999</v>
+      </c>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="6">
+        <f>ROUND(P6/P3,4)-1</f>
+        <v>0.70130000000000003</v>
+      </c>
+      <c r="S6" s="3">
+        <v>2.5127999999999999</v>
+      </c>
+      <c r="T6" s="7">
+        <f>ROUND(S6/S3,4)-1</f>
+        <v>0.47300000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="9"/>
+      <c r="O11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R11" s="11"/>
+    </row>
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="I12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2.6911999999999998</v>
+      </c>
+      <c r="L12" s="6">
+        <f>K12/M3-1</f>
+        <v>0.58017732370383412</v>
+      </c>
+      <c r="M12" s="2">
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="N12" s="6">
+        <f>M12/P3-1</f>
+        <v>0.59427904261529463</v>
+      </c>
+      <c r="O12" s="3">
+        <v>2.6671</v>
+      </c>
+      <c r="P12" s="6">
+        <f>O12/S3-1</f>
+        <v>0.56343625139687337</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>2.6861000000000002</v>
+      </c>
+      <c r="R12" s="6">
+        <f>Q12/U3-1</f>
+        <v>0.55122430122430122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1.9369000000000001</v>
+      </c>
+      <c r="L13" s="6">
+        <f>K13/M3-1</f>
+        <v>0.13727907932593508</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1.9479</v>
+      </c>
+      <c r="N13" s="6">
+        <f>M13/P3-1</f>
+        <v>0.13712784588441318</v>
+      </c>
+      <c r="O13" s="3">
+        <v>1.948</v>
+      </c>
+      <c r="P13" s="6">
+        <f>O13/S3-1</f>
+        <v>0.14190462214431743</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>1.9598</v>
+      </c>
+      <c r="R13" s="6">
+        <f>Q13/U3-1</f>
+        <v>0.13178563178563185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.9178999999999999</v>
+      </c>
+      <c r="L14" s="6">
+        <f>K14/M3-1</f>
+        <v>0.12612295226351944</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1.9254</v>
+      </c>
+      <c r="N14" s="6">
+        <f>M14/P3-1</f>
+        <v>0.1239929947460594</v>
+      </c>
+      <c r="O14" s="3">
+        <v>1.9054</v>
+      </c>
+      <c r="P14" s="6">
+        <f>O14/S3-1</f>
+        <v>0.11693278595163381</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="R14" s="6">
+        <f>Q14/U3-1</f>
+        <v>0.10533610533610527</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.8807</v>
+      </c>
+      <c r="L15" s="6">
+        <f>K15/M3-1</f>
+        <v>0.10428042980447416</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1.8951</v>
+      </c>
+      <c r="N15" s="6">
+        <f>M15/P3-1</f>
+        <v>0.10630472854640982</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1.8858999999999999</v>
+      </c>
+      <c r="P15" s="6">
+        <f>O15/S3-1</f>
+        <v>0.10550201586343344</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1.8766</v>
+      </c>
+      <c r="R15" s="6">
+        <f>Q15/U3-1</f>
+        <v>8.3737583737583776E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>3</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.8734</v>
+      </c>
+      <c r="L16" s="6">
+        <f>K16/M3-1</f>
+        <v>9.9994128354177647E-2</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1.8806</v>
+      </c>
+      <c r="N16" s="6">
+        <f>M16/P3-1</f>
+        <v>9.7840046701692884E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1.8732</v>
+      </c>
+      <c r="P16" s="6">
+        <f>O16/S3-1</f>
+        <v>9.8057360472656896E-2</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1.8537999999999999</v>
+      </c>
+      <c r="R16" s="6">
+        <f>Q16/U3-1</f>
+        <v>7.057057057057059E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>4</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.8678999999999999</v>
+      </c>
+      <c r="L17" s="6">
+        <f>K17/M3-1</f>
+        <v>9.6764723151899323E-2</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1.8741000000000001</v>
+      </c>
+      <c r="N17" s="6">
+        <f>M17/P3-1</f>
+        <v>9.4045534150613008E-2</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1.8652</v>
+      </c>
+      <c r="P17" s="6">
+        <f>O17/S3-1</f>
+        <v>9.3367813769805519E-2</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1.8504</v>
+      </c>
+      <c r="R17" s="6">
+        <f>Q17/U3-1</f>
+        <v>6.8607068607068555E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:T2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04364F8B-FA61-49FE-9A1A-9E99500FBC47}">
+  <dimension ref="A1:U17"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.140625" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" customWidth="1"/>
+    <col min="16" max="16" width="20.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" customWidth="1"/>
+    <col min="19" max="19" width="22" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" customWidth="1"/>
+    <col min="21" max="21" width="35.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="19"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="19"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="11"/>
+      <c r="U1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>104</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="19"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="11"/>
+      <c r="U2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="14">
+        <v>1.7073</v>
+      </c>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="14">
+        <v>1.7031000000000001</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="14">
+        <v>1.7130000000000001</v>
+      </c>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="17">
+        <v>1.7059218101262801</v>
+      </c>
+      <c r="T3" s="18"/>
+      <c r="U3" s="5">
+        <v>1.7116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3">
+        <v>136.69470000000001</v>
+      </c>
+      <c r="K4" s="20">
+        <f>ROUND(J4/J3,4)-1</f>
+        <v>79.064800000000005</v>
+      </c>
+      <c r="L4" s="21"/>
+      <c r="M4" s="10">
+        <v>132.49350000000001</v>
+      </c>
+      <c r="N4" s="11"/>
+      <c r="O4" s="7">
+        <f>ROUND(M4/M3,4)-1</f>
+        <v>76.795500000000004</v>
+      </c>
+      <c r="P4" s="10">
+        <v>151.20259999999999</v>
+      </c>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="6">
+        <f>ROUND(P4/P3,4)-1</f>
+        <v>87.267700000000005</v>
+      </c>
+      <c r="S4" s="3">
+        <v>49.514683496694197</v>
+      </c>
+      <c r="T4" s="7">
+        <f>ROUND(S4/S3,4)-1</f>
+        <v>28.025200000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2.5396999999999998</v>
+      </c>
+      <c r="K5" s="20">
+        <f>ROUND(J5/J3,4)-1</f>
+        <v>0.48760000000000003</v>
+      </c>
+      <c r="L5" s="21"/>
+      <c r="M5" s="10">
+        <v>2.5322</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5" s="7">
+        <f>ROUND(M5/M3,4)-1</f>
+        <v>0.4867999999999999</v>
+      </c>
+      <c r="P5" s="10">
+        <v>2.5428999999999999</v>
+      </c>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="6">
+        <f>ROUND(P5/P3,4)-1</f>
+        <v>0.48449999999999993</v>
+      </c>
+      <c r="S5" s="3">
+        <v>2.5407999999999999</v>
+      </c>
+      <c r="T5" s="7">
+        <f>ROUND(S5/S3,4)-1</f>
+        <v>0.48940000000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="I6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2.5535000000000001</v>
+      </c>
+      <c r="K6" s="20">
+        <f>ROUND(J6/J3,4)-1</f>
+        <v>0.49560000000000004</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="10">
+        <v>2.9327999999999999</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="7">
+        <f>ROUND(M6/M3,4)-1</f>
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="P6" s="10">
+        <v>2.9142999999999999</v>
+      </c>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="6">
+        <f>ROUND(P6/P3,4)-1</f>
+        <v>0.70130000000000003</v>
+      </c>
+      <c r="S6" s="3">
+        <v>2.5127999999999999</v>
+      </c>
+      <c r="T6" s="7">
+        <f>ROUND(S6/S3,4)-1</f>
+        <v>0.47300000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="I11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="9"/>
+      <c r="M11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="9"/>
+      <c r="O11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="R11" s="11"/>
+    </row>
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="I12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2.6911999999999998</v>
+      </c>
+      <c r="L12" s="6">
+        <f>K12/M3-1</f>
+        <v>0.58017732370383412</v>
+      </c>
+      <c r="M12" s="2">
+        <v>2.7309999999999999</v>
+      </c>
+      <c r="N12" s="6">
+        <f>M12/P3-1</f>
+        <v>0.59427904261529463</v>
+      </c>
+      <c r="O12" s="3">
+        <v>2.6671</v>
+      </c>
+      <c r="P12" s="6">
+        <f>O12/S3-1</f>
+        <v>0.56343625139687337</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>2.6861000000000002</v>
+      </c>
+      <c r="R12" s="6">
+        <f>Q12/U3-1</f>
+        <v>0.56935031549427451</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1.9369000000000001</v>
+      </c>
+      <c r="L13" s="6">
+        <f>K13/M3-1</f>
+        <v>0.13727907932593508</v>
+      </c>
+      <c r="M13" s="3">
+        <v>1.9479</v>
+      </c>
+      <c r="N13" s="6">
+        <f>M13/P3-1</f>
+        <v>0.13712784588441318</v>
+      </c>
+      <c r="O13" s="3">
+        <v>1.948</v>
+      </c>
+      <c r="P13" s="6">
+        <f>O13/S3-1</f>
+        <v>0.14190462214431743</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>1.9527000000000001</v>
+      </c>
+      <c r="R13" s="6">
+        <f>Q13/U3-1</f>
+        <v>0.14086235101659272</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I14" s="2">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.9159999999999999</v>
+      </c>
+      <c r="L14" s="6">
+        <f>K14/M3-1</f>
+        <v>0.12500733955727772</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1.9268000000000001</v>
+      </c>
+      <c r="N14" s="6">
+        <f>M14/P3-1</f>
+        <v>0.12481027437244596</v>
+      </c>
+      <c r="O14" s="3">
+        <v>1.9142999999999999</v>
+      </c>
+      <c r="P14" s="6">
+        <f>O14/S3-1</f>
+        <v>0.12214990665855585</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>1.9112</v>
+      </c>
+      <c r="R14" s="6">
+        <f>Q14/U3-1</f>
+        <v>0.11661603178312685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I15" s="2">
+        <v>2</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.8943000000000001</v>
+      </c>
+      <c r="L15" s="6">
+        <f>K15/M3-1</f>
+        <v>0.11226586812283479</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1.8937999999999999</v>
+      </c>
+      <c r="N15" s="6">
+        <f>M15/P3-1</f>
+        <v>0.10554582603619367</v>
+      </c>
+      <c r="O15" s="2">
+        <v>1.8992</v>
+      </c>
+      <c r="P15" s="6">
+        <f>O15/S3-1</f>
+        <v>0.11329838725692398</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>1.8764000000000001</v>
+      </c>
+      <c r="R15" s="6">
+        <f>Q15/U3-1</f>
+        <v>9.6284178546389487E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="I16" s="2">
+        <v>3</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.8933</v>
+      </c>
+      <c r="L16" s="6">
+        <f>K16/M3-1</f>
+        <v>0.11167870354060239</v>
+      </c>
+      <c r="M16" s="2">
+        <v>1.899</v>
+      </c>
+      <c r="N16" s="6">
+        <f>M16/P3-1</f>
+        <v>0.10858143607705784</v>
+      </c>
+      <c r="O16" s="2">
+        <v>1.8916999999999999</v>
+      </c>
+      <c r="P16" s="6">
+        <f>O16/S3-1</f>
+        <v>0.10890193722300068</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>1.8633999999999999</v>
+      </c>
+      <c r="R16" s="6">
+        <f>Q16/U3-1</f>
+        <v>8.8688946015424097E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="9:18" x14ac:dyDescent="0.25">
+      <c r="I17" s="2">
+        <v>4</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1.8993</v>
+      </c>
+      <c r="L17" s="6">
+        <f>K17/M3-1</f>
+        <v>0.1152016910339968</v>
+      </c>
+      <c r="M17" s="2">
+        <v>1.9074</v>
+      </c>
+      <c r="N17" s="6">
+        <f>M17/P3-1</f>
+        <v>0.11348511383537652</v>
+      </c>
+      <c r="O17" s="3">
+        <v>1.8976999999999999</v>
+      </c>
+      <c r="P17" s="6">
+        <f>O17/S3-1</f>
+        <v>0.11241909725013932</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1.8581000000000001</v>
+      </c>
+      <c r="R17" s="6">
+        <f>Q17/U3-1</f>
+        <v>8.5592428137415411E-2</v>
       </c>
     </row>
   </sheetData>
@@ -9394,12 +10408,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EDA6A5E-47CB-4971-B4D4-80E7225292CB}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412146B7-669A-4A41-83DA-A8A466CECDDE}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="O1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9408,524 +10422,15 @@
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" customWidth="1"/>
-    <col min="19" max="19" width="22" customWidth="1"/>
-    <col min="20" max="20" width="24.5703125" customWidth="1"/>
-    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>34</v>
-      </c>
-      <c r="B2">
-        <v>104</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="T2" s="10"/>
-      <c r="U2" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="I3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="11">
-        <v>1.7073</v>
-      </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="11">
-        <v>1.7031000000000001</v>
-      </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="11">
-        <v>1.7130000000000001</v>
-      </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="14">
-        <v>1.7059218101262801</v>
-      </c>
-      <c r="T3" s="15"/>
-      <c r="U3" s="5">
-        <v>1.7316</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="3">
-        <v>136.69470000000001</v>
-      </c>
-      <c r="K4" s="20">
-        <f>ROUND(J4/J3,4)-1</f>
-        <v>79.064800000000005</v>
-      </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="8">
-        <v>132.49350000000001</v>
-      </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="7">
-        <f>ROUND(M4/M3,4)-1</f>
-        <v>76.795500000000004</v>
-      </c>
-      <c r="P4" s="8">
-        <v>151.20259999999999</v>
-      </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="6">
-        <f>ROUND(P4/P3,4)-1</f>
-        <v>87.267700000000005</v>
-      </c>
-      <c r="S4" s="3">
-        <v>49.514683496694197</v>
-      </c>
-      <c r="T4" s="7">
-        <f>ROUND(S4/S3,4)-1</f>
-        <v>28.025200000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="3">
-        <v>2.5396999999999998</v>
-      </c>
-      <c r="K5" s="20">
-        <f>ROUND(J5/J3,4)-1</f>
-        <v>0.48760000000000003</v>
-      </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="8">
-        <v>2.5322</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="7">
-        <f>ROUND(M5/M3,4)-1</f>
-        <v>0.4867999999999999</v>
-      </c>
-      <c r="P5" s="8">
-        <v>2.5428999999999999</v>
-      </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="6">
-        <f>ROUND(P5/P3,4)-1</f>
-        <v>0.48449999999999993</v>
-      </c>
-      <c r="S5" s="3">
-        <v>2.5407999999999999</v>
-      </c>
-      <c r="T5" s="7">
-        <f>ROUND(S5/S3,4)-1</f>
-        <v>0.48940000000000006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="I6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="3">
-        <v>2.5535000000000001</v>
-      </c>
-      <c r="K6" s="20">
-        <f>ROUND(J6/J3,4)-1</f>
-        <v>0.49560000000000004</v>
-      </c>
-      <c r="L6" s="21"/>
-      <c r="M6" s="8">
-        <v>2.9327999999999999</v>
-      </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="7">
-        <f>ROUND(M6/M3,4)-1</f>
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="P6" s="8">
-        <v>2.9142999999999999</v>
-      </c>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="6">
-        <f>ROUND(P6/P3,4)-1</f>
-        <v>0.70130000000000003</v>
-      </c>
-      <c r="S6" s="3">
-        <v>2.5127999999999999</v>
-      </c>
-      <c r="T6" s="7">
-        <f>ROUND(S6/S3,4)-1</f>
-        <v>0.47300000000000009</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="I11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="10"/>
-    </row>
-    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="I12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="2">
-        <v>2.6836000000000002</v>
-      </c>
-      <c r="L12" s="6">
-        <f>K12/M3-1</f>
-        <v>0.57571487287886791</v>
-      </c>
-      <c r="M12" s="2">
-        <v>2.7757999999999998</v>
-      </c>
-      <c r="N12" s="6">
-        <f>M12/P3-1</f>
-        <v>0.62043199065966115</v>
-      </c>
-      <c r="O12" s="3">
-        <v>2.6745000000000001</v>
-      </c>
-      <c r="P12" s="6">
-        <f>O12/S3-1</f>
-        <v>0.56777408209701097</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>2.7198000000000002</v>
-      </c>
-      <c r="R12" s="6">
-        <f>Q12/U3-1</f>
-        <v>0.5706860706860708</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="3">
-        <v>1.9369000000000001</v>
-      </c>
-      <c r="L13" s="6">
-        <f>K13/M3-1</f>
-        <v>0.13727907932593508</v>
-      </c>
-      <c r="M13" s="3">
-        <v>1.9479</v>
-      </c>
-      <c r="N13" s="6">
-        <f>M13/P3-1</f>
-        <v>0.13712784588441318</v>
-      </c>
-      <c r="O13" s="3">
-        <v>1.948</v>
-      </c>
-      <c r="P13" s="6">
-        <f>O13/S3-1</f>
-        <v>0.14190462214431743</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>1.9598</v>
-      </c>
-      <c r="R13" s="6">
-        <f>Q13/U3-1</f>
-        <v>0.13178563178563185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1.9178999999999999</v>
-      </c>
-      <c r="L14" s="6">
-        <f>K14/M3-1</f>
-        <v>0.12612295226351944</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1.9254</v>
-      </c>
-      <c r="N14" s="6">
-        <f>M14/P3-1</f>
-        <v>0.1239929947460594</v>
-      </c>
-      <c r="O14" s="3">
-        <v>1.9054</v>
-      </c>
-      <c r="P14" s="6">
-        <f>O14/S3-1</f>
-        <v>0.11693278595163381</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>1.9139999999999999</v>
-      </c>
-      <c r="R14" s="6">
-        <f>Q14/U3-1</f>
-        <v>0.10533610533610527</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I15" s="2">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1.8807</v>
-      </c>
-      <c r="L15" s="6">
-        <f>K15/M3-1</f>
-        <v>0.10428042980447416</v>
-      </c>
-      <c r="M15" s="2">
-        <v>1.8951</v>
-      </c>
-      <c r="N15" s="6">
-        <f>M15/P3-1</f>
-        <v>0.10630472854640982</v>
-      </c>
-      <c r="O15" s="2">
-        <v>1.8858999999999999</v>
-      </c>
-      <c r="P15" s="6">
-        <f>O15/S3-1</f>
-        <v>0.10550201586343344</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>1.8766</v>
-      </c>
-      <c r="R15" s="6">
-        <f>Q15/U3-1</f>
-        <v>8.3737583737583776E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I16" s="2">
-        <v>3</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1.8734</v>
-      </c>
-      <c r="L16" s="6">
-        <f>K16/M3-1</f>
-        <v>9.9994128354177647E-2</v>
-      </c>
-      <c r="M16" s="2">
-        <v>1.8806</v>
-      </c>
-      <c r="N16" s="6">
-        <f>M16/P3-1</f>
-        <v>9.7840046701692884E-2</v>
-      </c>
-      <c r="O16" s="2">
-        <v>1.8732</v>
-      </c>
-      <c r="P16" s="6">
-        <f>O16/S3-1</f>
-        <v>9.8057360472656896E-2</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>1.8537999999999999</v>
-      </c>
-      <c r="R16" s="6">
-        <f>Q16/U3-1</f>
-        <v>7.057057057057059E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I17" s="2">
-        <v>4</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1.8678999999999999</v>
-      </c>
-      <c r="L17" s="6">
-        <f>K17/M3-1</f>
-        <v>9.6764723151899323E-2</v>
-      </c>
-      <c r="M17" s="2">
-        <v>1.8741000000000001</v>
-      </c>
-      <c r="N17" s="6">
-        <f>M17/P3-1</f>
-        <v>9.4045534150613008E-2</v>
-      </c>
-      <c r="O17" s="3">
-        <v>1.8652</v>
-      </c>
-      <c r="P17" s="6">
-        <f>O17/S3-1</f>
-        <v>9.3367813769805519E-2</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1.8504</v>
-      </c>
-      <c r="R17" s="6">
-        <f>Q17/U3-1</f>
-        <v>6.8607068607068555E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="P6:Q6"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04364F8B-FA61-49FE-9A1A-9E99500FBC47}">
-  <dimension ref="A1:U17"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R21" sqref="R21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.140625" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
-    <col min="14" max="14" width="18" customWidth="1"/>
-    <col min="15" max="15" width="25.85546875" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" customWidth="1"/>
-    <col min="19" max="19" width="22" customWidth="1"/>
-    <col min="20" max="20" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="43.42578125" customWidth="1"/>
+    <col min="11" max="11" width="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="36" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" customWidth="1"/>
+    <col min="17" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="20.42578125" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" customWidth="1"/>
+    <col min="20" max="20" width="28.85546875" customWidth="1"/>
     <col min="21" max="21" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9940,61 +10445,61 @@
         <v>2</v>
       </c>
       <c r="I1" s="3"/>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="8" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="8" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="8" t="s">
+      <c r="Q1" s="19"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="10"/>
+      <c r="T1" s="11"/>
       <c r="U1" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="8" t="s">
+      <c r="N2" s="19"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="8" t="s">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="10"/>
+      <c r="T2" s="11"/>
       <c r="U2" s="3" t="s">
         <v>6</v>
       </c>
@@ -10003,27 +10508,28 @@
       <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="11">
-        <v>1.7073</v>
-      </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="11">
-        <v>1.7031000000000001</v>
-      </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="11">
-        <v>1.7130000000000001</v>
-      </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
+      <c r="J3" s="14">
+        <f>ROUND(1.3137349069022,4)</f>
+        <v>1.3137000000000001</v>
+      </c>
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="14">
+        <v>1.3108</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="14">
+        <v>1.3133999999999999</v>
+      </c>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
       <c r="S3" s="14">
-        <v>1.7059218101262801</v>
-      </c>
-      <c r="T3" s="15"/>
+        <v>1.3113999999999999</v>
+      </c>
+      <c r="T3" s="16"/>
       <c r="U3" s="5">
-        <v>1.7116</v>
+        <v>1.3261000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -10031,35 +10537,36 @@
         <v>10</v>
       </c>
       <c r="J4" s="3">
-        <v>136.69470000000001</v>
-      </c>
-      <c r="K4" s="20">
+        <f>ROUND(1.88295256877831,4)</f>
+        <v>1.883</v>
+      </c>
+      <c r="K4" s="12">
         <f>ROUND(J4/J3,4)-1</f>
-        <v>79.064800000000005</v>
-      </c>
-      <c r="L4" s="21"/>
-      <c r="M4" s="8">
-        <v>132.49350000000001</v>
-      </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="7">
+        <v>0.43340000000000001</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="10">
+        <v>1.9887999999999999</v>
+      </c>
+      <c r="N4" s="11"/>
+      <c r="O4" s="6">
         <f>ROUND(M4/M3,4)-1</f>
-        <v>76.795500000000004</v>
-      </c>
-      <c r="P4" s="8">
-        <v>151.20259999999999</v>
-      </c>
-      <c r="Q4" s="10"/>
+        <v>0.5172000000000001</v>
+      </c>
+      <c r="P4" s="10">
+        <v>1.8765000000000001</v>
+      </c>
+      <c r="Q4" s="11"/>
       <c r="R4" s="6">
         <f>ROUND(P4/P3,4)-1</f>
-        <v>87.267700000000005</v>
+        <v>0.42870000000000008</v>
       </c>
       <c r="S4" s="3">
-        <v>49.514683496694197</v>
-      </c>
-      <c r="T4" s="7">
+        <v>1.8301000000000001</v>
+      </c>
+      <c r="T4" s="6">
         <f>ROUND(S4/S3,4)-1</f>
-        <v>28.025200000000002</v>
+        <v>0.39549999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -10067,35 +10574,35 @@
         <v>11</v>
       </c>
       <c r="J5" s="3">
-        <v>2.5396999999999998</v>
-      </c>
-      <c r="K5" s="20">
+        <v>1.6628000000000001</v>
+      </c>
+      <c r="K5" s="12">
         <f>ROUND(J5/J3,4)-1</f>
-        <v>0.48760000000000003</v>
-      </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="8">
-        <v>2.5322</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="7">
+        <v>0.26570000000000005</v>
+      </c>
+      <c r="L5" s="13"/>
+      <c r="M5" s="10">
+        <v>1.661</v>
+      </c>
+      <c r="N5" s="11"/>
+      <c r="O5" s="6">
         <f>ROUND(M5/M3,4)-1</f>
-        <v>0.4867999999999999</v>
-      </c>
-      <c r="P5" s="8">
-        <v>2.5428999999999999</v>
-      </c>
-      <c r="Q5" s="10"/>
+        <v>0.2672000000000001</v>
+      </c>
+      <c r="P5" s="10">
+        <v>1.6674</v>
+      </c>
+      <c r="Q5" s="11"/>
       <c r="R5" s="6">
         <f>ROUND(P5/P3,4)-1</f>
-        <v>0.48449999999999993</v>
+        <v>0.26950000000000007</v>
       </c>
       <c r="S5" s="3">
-        <v>2.5407999999999999</v>
-      </c>
-      <c r="T5" s="7">
+        <v>1.6593</v>
+      </c>
+      <c r="T5" s="6">
         <f>ROUND(S5/S3,4)-1</f>
-        <v>0.48940000000000006</v>
+        <v>0.26530000000000009</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -10103,60 +10610,60 @@
         <v>12</v>
       </c>
       <c r="J6" s="3">
-        <v>2.5535000000000001</v>
-      </c>
-      <c r="K6" s="20">
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="K6" s="12">
         <f>ROUND(J6/J3,4)-1</f>
-        <v>0.49560000000000004</v>
-      </c>
-      <c r="L6" s="21"/>
-      <c r="M6" s="8">
-        <v>2.9327999999999999</v>
-      </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="7">
+        <v>0.29940000000000011</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="10">
+        <v>1.6947000000000001</v>
+      </c>
+      <c r="N6" s="11"/>
+      <c r="O6" s="6">
         <f>ROUND(M6/M3,4)-1</f>
-        <v>0.72199999999999998</v>
-      </c>
-      <c r="P6" s="8">
-        <v>2.9142999999999999</v>
-      </c>
-      <c r="Q6" s="10"/>
+        <v>0.29289999999999994</v>
+      </c>
+      <c r="P6" s="10">
+        <v>1.7579</v>
+      </c>
+      <c r="Q6" s="11"/>
       <c r="R6" s="6">
         <f>ROUND(P6/P3,4)-1</f>
-        <v>0.70130000000000003</v>
+        <v>0.33840000000000003</v>
       </c>
       <c r="S6" s="3">
-        <v>2.5127999999999999</v>
-      </c>
-      <c r="T6" s="7">
+        <v>1.7423999999999999</v>
+      </c>
+      <c r="T6" s="6">
         <f>ROUND(S6/S3,4)-1</f>
-        <v>0.47300000000000009</v>
+        <v>0.32869999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="I11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="18" t="s">
+      <c r="L11" s="9"/>
+      <c r="M11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="8" t="s">
+      <c r="N11" s="9"/>
+      <c r="O11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="8" t="s">
+      <c r="P11" s="11"/>
+      <c r="Q11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="10"/>
+      <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="I12" s="2" t="s">
@@ -10166,32 +10673,32 @@
         <v>15</v>
       </c>
       <c r="K12" s="2">
-        <v>2.6836000000000002</v>
+        <v>1.6334</v>
       </c>
       <c r="L12" s="6">
         <f>K12/M3-1</f>
-        <v>0.57571487287886791</v>
+        <v>0.24610924626182484</v>
       </c>
       <c r="M12" s="2">
-        <v>2.7757999999999998</v>
+        <v>1.6202000000000001</v>
       </c>
       <c r="N12" s="6">
         <f>M12/P3-1</f>
-        <v>0.62043199065966115</v>
+        <v>0.23359220344144993</v>
       </c>
       <c r="O12" s="3">
-        <v>2.6745000000000001</v>
+        <v>1.6294999999999999</v>
       </c>
       <c r="P12" s="6">
         <f>O12/S3-1</f>
-        <v>0.56777408209701097</v>
+        <v>0.2425651974988563</v>
       </c>
       <c r="Q12" s="3">
-        <v>2.6947999999999999</v>
+        <v>1.641</v>
       </c>
       <c r="R12" s="6">
         <f>Q12/U3-1</f>
-        <v>0.57443327880345874</v>
+        <v>0.23746323806651071</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -10202,32 +10709,32 @@
         <v>15</v>
       </c>
       <c r="K13" s="3">
-        <v>1.9369000000000001</v>
+        <v>1.5123</v>
       </c>
       <c r="L13" s="6">
         <f>K13/M3-1</f>
-        <v>0.13727907932593508</v>
+        <v>0.15372291730241083</v>
       </c>
       <c r="M13" s="3">
-        <v>1.9479</v>
+        <v>1.5193000000000001</v>
       </c>
       <c r="N13" s="6">
         <f>M13/P3-1</f>
-        <v>0.13712784588441318</v>
+        <v>0.15676869194457144</v>
       </c>
       <c r="O13" s="3">
-        <v>1.948</v>
+        <v>1.5106999999999999</v>
       </c>
       <c r="P13" s="6">
         <f>O13/S3-1</f>
-        <v>0.14190462214431743</v>
+        <v>0.15197498856184244</v>
       </c>
       <c r="Q13" s="3">
-        <v>1.9527000000000001</v>
+        <v>1.5098</v>
       </c>
       <c r="R13" s="6">
         <f>Q13/U3-1</f>
-        <v>0.14086235101659272</v>
+        <v>0.13852650629665941</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -10235,35 +10742,35 @@
         <v>1</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="K14" s="2">
-        <v>1.9159999999999999</v>
+        <v>1.5014000000000001</v>
       </c>
       <c r="L14" s="6">
         <f>K14/M3-1</f>
-        <v>0.12500733955727772</v>
+        <v>0.14540738480317361</v>
       </c>
       <c r="M14" s="2">
-        <v>1.9268000000000001</v>
+        <v>1.4993000000000001</v>
       </c>
       <c r="N14" s="6">
         <f>M14/P3-1</f>
-        <v>0.12481027437244596</v>
+        <v>0.14154103852596323</v>
       </c>
       <c r="O14" s="3">
-        <v>1.9142999999999999</v>
+        <v>1.502</v>
       </c>
       <c r="P14" s="6">
         <f>O14/S3-1</f>
-        <v>0.12214990665855585</v>
+        <v>0.14534085709928335</v>
       </c>
       <c r="Q14" s="3">
-        <v>1.9112</v>
+        <v>1.4966999999999999</v>
       </c>
       <c r="R14" s="6">
         <f>Q14/U3-1</f>
-        <v>0.11661603178312685</v>
+        <v>0.12864791493854155</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -10271,35 +10778,35 @@
         <v>2</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K15" s="2">
-        <v>1.8943000000000001</v>
+        <v>1.4744999999999999</v>
       </c>
       <c r="L15" s="6">
         <f>K15/M3-1</f>
-        <v>0.11226586812283479</v>
+        <v>0.12488556606652423</v>
       </c>
       <c r="M15" s="2">
-        <v>1.8937999999999999</v>
+        <v>1.4734</v>
       </c>
       <c r="N15" s="6">
         <f>M15/P3-1</f>
-        <v>0.10554582603619367</v>
+        <v>0.12182122734886569</v>
       </c>
       <c r="O15" s="2">
-        <v>1.8992</v>
+        <v>1.4752000000000001</v>
       </c>
       <c r="P15" s="6">
         <f>O15/S3-1</f>
-        <v>0.11329838725692398</v>
+        <v>0.12490468201921634</v>
       </c>
       <c r="Q15" s="2">
-        <v>1.8764000000000001</v>
+        <v>1.4653</v>
       </c>
       <c r="R15" s="6">
         <f>Q15/U3-1</f>
-        <v>9.6284178546389487E-2</v>
+        <v>0.10496945931679358</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -10307,35 +10814,35 @@
         <v>3</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="K16" s="2">
-        <v>1.8933</v>
+        <v>1.4461999999999999</v>
       </c>
       <c r="L16" s="6">
         <f>K16/M3-1</f>
-        <v>0.11167870354060239</v>
+        <v>0.10329569728410126</v>
       </c>
       <c r="M16" s="2">
-        <v>1.899</v>
+        <v>1.4498</v>
       </c>
       <c r="N16" s="6">
         <f>M16/P3-1</f>
-        <v>0.10858143607705784</v>
+        <v>0.10385259631490795</v>
       </c>
       <c r="O16" s="2">
-        <v>1.8916999999999999</v>
+        <v>1.4549000000000001</v>
       </c>
       <c r="P16" s="6">
         <f>O16/S3-1</f>
-        <v>0.10890193722300068</v>
-      </c>
-      <c r="Q16" s="2">
-        <v>1.8633999999999999</v>
+        <v>0.10942504193991165</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1.4409000000000001</v>
       </c>
       <c r="R16" s="6">
         <f>Q16/U3-1</f>
-        <v>8.8688946015424097E-2</v>
+        <v>8.6569640298620021E-2</v>
       </c>
     </row>
     <row r="17" spans="9:18" x14ac:dyDescent="0.25">
@@ -10343,35 +10850,35 @@
         <v>4</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="K17" s="2">
-        <v>1.8993</v>
+        <v>1.44</v>
       </c>
       <c r="L17" s="6">
         <f>K17/M3-1</f>
-        <v>0.1152016910339968</v>
+        <v>9.8565761367104043E-2</v>
       </c>
       <c r="M17" s="2">
-        <v>1.9074</v>
+        <v>1.4302999999999999</v>
       </c>
       <c r="N17" s="6">
         <f>M17/P3-1</f>
-        <v>0.11348511383537652</v>
+        <v>8.9005634231764885E-2</v>
       </c>
       <c r="O17" s="3">
-        <v>1.8976999999999999</v>
+        <v>1.427</v>
       </c>
       <c r="P17" s="6">
         <f>O17/S3-1</f>
-        <v>0.11241909725013932</v>
+        <v>8.8150068628946254E-2</v>
       </c>
       <c r="Q17" s="3">
-        <v>1.8581000000000001</v>
+        <v>1.4093</v>
       </c>
       <c r="R17" s="6">
         <f>Q17/U3-1</f>
-        <v>8.5592428137415411E-2</v>
+        <v>6.2740366488198474E-2</v>
       </c>
     </row>
   </sheetData>
@@ -10403,513 +10910,6 @@
     <mergeCell ref="Q11:R11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412146B7-669A-4A41-83DA-A8A466CECDDE}">
-  <dimension ref="A1:U17"/>
-  <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="43.42578125" customWidth="1"/>
-    <col min="11" max="11" width="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="36" customWidth="1"/>
-    <col min="15" max="15" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="30.42578125" customWidth="1"/>
-    <col min="17" max="17" width="12" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
-    <col min="20" max="20" width="28.85546875" customWidth="1"/>
-    <col min="21" max="21" width="35.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>86</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="T2" s="10"/>
-      <c r="U2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="I3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="11">
-        <f>ROUND(1.3137349069022,4)</f>
-        <v>1.3137000000000001</v>
-      </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="11">
-        <v>1.3108</v>
-      </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="11">
-        <v>1.3133999999999999</v>
-      </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="11">
-        <v>1.3113999999999999</v>
-      </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="5">
-        <v>1.3261000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="3">
-        <f>ROUND(1.88295256877831,4)</f>
-        <v>1.883</v>
-      </c>
-      <c r="K4" s="16">
-        <f>ROUND(J4/J3,4)-1</f>
-        <v>0.43340000000000001</v>
-      </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="8">
-        <v>1.9887999999999999</v>
-      </c>
-      <c r="N4" s="10"/>
-      <c r="O4" s="6">
-        <f>ROUND(M4/M3,4)-1</f>
-        <v>0.5172000000000001</v>
-      </c>
-      <c r="P4" s="8">
-        <v>1.8765000000000001</v>
-      </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="6">
-        <f>ROUND(P4/P3,4)-1</f>
-        <v>0.42870000000000008</v>
-      </c>
-      <c r="S4" s="3">
-        <v>1.8301000000000001</v>
-      </c>
-      <c r="T4" s="6">
-        <f>ROUND(S4/S3,4)-1</f>
-        <v>0.39549999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1.6628000000000001</v>
-      </c>
-      <c r="K5" s="16">
-        <f>ROUND(J5/J3,4)-1</f>
-        <v>0.26570000000000005</v>
-      </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="8">
-        <v>1.661</v>
-      </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="6">
-        <f>ROUND(M5/M3,4)-1</f>
-        <v>0.2672000000000001</v>
-      </c>
-      <c r="P5" s="8">
-        <v>1.6674</v>
-      </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="6">
-        <f>ROUND(P5/P3,4)-1</f>
-        <v>0.26950000000000007</v>
-      </c>
-      <c r="S5" s="3">
-        <v>1.6593</v>
-      </c>
-      <c r="T5" s="6">
-        <f>ROUND(S5/S3,4)-1</f>
-        <v>0.26530000000000009</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="I6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="3">
-        <v>1.7070000000000001</v>
-      </c>
-      <c r="K6" s="16">
-        <f>ROUND(J6/J3,4)-1</f>
-        <v>0.29940000000000011</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="8">
-        <v>1.6947000000000001</v>
-      </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="6">
-        <f>ROUND(M6/M3,4)-1</f>
-        <v>0.29289999999999994</v>
-      </c>
-      <c r="P6" s="8">
-        <v>1.7579</v>
-      </c>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="6">
-        <f>ROUND(P6/P3,4)-1</f>
-        <v>0.33840000000000003</v>
-      </c>
-      <c r="S6" s="3">
-        <v>1.7423999999999999</v>
-      </c>
-      <c r="T6" s="6">
-        <f>ROUND(S6/S3,4)-1</f>
-        <v>0.32869999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="R11" s="10"/>
-    </row>
-    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="I12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1.6414</v>
-      </c>
-      <c r="L12" s="6">
-        <f>K12/M3-1</f>
-        <v>0.25221238938053103</v>
-      </c>
-      <c r="M12" s="2">
-        <v>1.6188</v>
-      </c>
-      <c r="N12" s="6">
-        <f>M12/P3-1</f>
-        <v>0.23252626770214713</v>
-      </c>
-      <c r="O12" s="3">
-        <v>1.633</v>
-      </c>
-      <c r="P12" s="6">
-        <f>O12/S3-1</f>
-        <v>0.24523410096080545</v>
-      </c>
-      <c r="Q12" s="3">
-        <v>1.6323000000000001</v>
-      </c>
-      <c r="R12" s="6">
-        <f>Q12/U3-1</f>
-        <v>0.23090264685921125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="3">
-        <v>1.5123</v>
-      </c>
-      <c r="L13" s="6">
-        <f>K13/M3-1</f>
-        <v>0.15372291730241083</v>
-      </c>
-      <c r="M13" s="3">
-        <v>1.5193000000000001</v>
-      </c>
-      <c r="N13" s="6">
-        <f>M13/P3-1</f>
-        <v>0.15676869194457144</v>
-      </c>
-      <c r="O13" s="3">
-        <v>1.5106999999999999</v>
-      </c>
-      <c r="P13" s="6">
-        <f>O13/S3-1</f>
-        <v>0.15197498856184244</v>
-      </c>
-      <c r="Q13" s="3">
-        <v>1.5098</v>
-      </c>
-      <c r="R13" s="6">
-        <f>Q13/U3-1</f>
-        <v>0.13852650629665941</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I14" s="2">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1.5014000000000001</v>
-      </c>
-      <c r="L14" s="6">
-        <f>K14/M3-1</f>
-        <v>0.14540738480317361</v>
-      </c>
-      <c r="M14" s="2">
-        <v>1.4993000000000001</v>
-      </c>
-      <c r="N14" s="6">
-        <f>M14/P3-1</f>
-        <v>0.14154103852596323</v>
-      </c>
-      <c r="O14" s="3">
-        <v>1.502</v>
-      </c>
-      <c r="P14" s="6">
-        <f>O14/S3-1</f>
-        <v>0.14534085709928335</v>
-      </c>
-      <c r="Q14" s="3">
-        <v>1.4966999999999999</v>
-      </c>
-      <c r="R14" s="6">
-        <f>Q14/U3-1</f>
-        <v>0.12864791493854155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I15" s="2">
-        <v>2</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1.4744999999999999</v>
-      </c>
-      <c r="L15" s="6">
-        <f>K15/M3-1</f>
-        <v>0.12488556606652423</v>
-      </c>
-      <c r="M15" s="2">
-        <v>1.4734</v>
-      </c>
-      <c r="N15" s="6">
-        <f>M15/P3-1</f>
-        <v>0.12182122734886569</v>
-      </c>
-      <c r="O15" s="2">
-        <v>1.4752000000000001</v>
-      </c>
-      <c r="P15" s="6">
-        <f>O15/S3-1</f>
-        <v>0.12490468201921634</v>
-      </c>
-      <c r="Q15" s="2">
-        <v>1.4653</v>
-      </c>
-      <c r="R15" s="6">
-        <f>Q15/U3-1</f>
-        <v>0.10496945931679358</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="I16" s="2">
-        <v>3</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16" s="2">
-        <v>1.4461999999999999</v>
-      </c>
-      <c r="L16" s="6">
-        <f>K16/M3-1</f>
-        <v>0.10329569728410126</v>
-      </c>
-      <c r="M16" s="2">
-        <v>1.4498</v>
-      </c>
-      <c r="N16" s="6">
-        <f>M16/P3-1</f>
-        <v>0.10385259631490795</v>
-      </c>
-      <c r="O16" s="2">
-        <v>1.4549000000000001</v>
-      </c>
-      <c r="P16" s="6">
-        <f>O16/S3-1</f>
-        <v>0.10942504193991165</v>
-      </c>
-      <c r="Q16" s="3">
-        <v>1.4409000000000001</v>
-      </c>
-      <c r="R16" s="6">
-        <f>Q16/U3-1</f>
-        <v>8.6569640298620021E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="9:18" x14ac:dyDescent="0.25">
-      <c r="I17" s="2">
-        <v>4</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1.44</v>
-      </c>
-      <c r="L17" s="6">
-        <f>K17/M3-1</f>
-        <v>9.8565761367104043E-2</v>
-      </c>
-      <c r="M17" s="2">
-        <v>1.4302999999999999</v>
-      </c>
-      <c r="N17" s="6">
-        <f>M17/P3-1</f>
-        <v>8.9005634231764885E-2</v>
-      </c>
-      <c r="O17" s="3">
-        <v>1.427</v>
-      </c>
-      <c r="P17" s="6">
-        <f>O17/S3-1</f>
-        <v>8.8150068628946254E-2</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>1.4093</v>
-      </c>
-      <c r="R17" s="6">
-        <f>Q17/U3-1</f>
-        <v>6.2740366488198474E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:T2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -10920,7 +10920,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView topLeftCell="K1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10952,25 +10952,25 @@
         <v>2</v>
       </c>
       <c r="I1" s="3"/>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="8" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="8" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="8" t="s">
+      <c r="Q1" s="19"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="10"/>
+      <c r="T1" s="11"/>
       <c r="U1" s="3" t="s">
         <v>7</v>
       </c>
@@ -10988,25 +10988,25 @@
       <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="8" t="s">
+      <c r="N2" s="19"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="8" t="s">
+      <c r="Q2" s="19"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="T2" s="10"/>
+      <c r="T2" s="11"/>
       <c r="U2" s="3" t="s">
         <v>6</v>
       </c>
@@ -11015,29 +11015,29 @@
       <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="14">
         <f>ROUND(1.04953105339334,4)</f>
         <v>1.0495000000000001</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="11">
+      <c r="K3" s="15"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="14">
         <f>ROUND(1.04960738441608,4)</f>
         <v>1.0496000000000001</v>
       </c>
-      <c r="N3" s="12"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="11">
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="14">
         <f>ROUND(1.04726929636432,4)</f>
         <v>1.0472999999999999</v>
       </c>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="11">
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="14">
         <f>ROUND(1.05010333606256,4)</f>
         <v>1.0501</v>
       </c>
-      <c r="T3" s="13"/>
+      <c r="T3" s="16"/>
       <c r="U3" s="5">
         <f>ROUND(1.0532225410055,4)</f>
         <v>1.0531999999999999</v>
@@ -11051,25 +11051,25 @@
         <f>ROUND(1.29359759152171,4)</f>
         <v>1.2936000000000001</v>
       </c>
-      <c r="K4" s="16">
+      <c r="K4" s="12">
         <f>ROUND(J4/J3,4)-1</f>
         <v>0.23259999999999992</v>
       </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="8">
+      <c r="L4" s="13"/>
+      <c r="M4" s="10">
         <f>ROUND(1.32368411192381,4)</f>
         <v>1.3237000000000001</v>
       </c>
-      <c r="N4" s="10"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="6">
         <f>ROUND(M4/M3,4)-1</f>
         <v>0.26110000000000011</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="10">
         <f>ROUND(1.29757323247913,4)</f>
         <v>1.2976000000000001</v>
       </c>
-      <c r="Q4" s="10"/>
+      <c r="Q4" s="11"/>
       <c r="R4" s="6">
         <f>ROUND(P4/P3,4)-1</f>
         <v>0.2390000000000001</v>
@@ -11090,23 +11090,23 @@
       <c r="J5" s="3">
         <v>1.2487999999999999</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="12">
         <f>ROUND(J5/J3,4)-1</f>
         <v>0.18989999999999996</v>
       </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="8">
+      <c r="L5" s="13"/>
+      <c r="M5" s="10">
         <v>1.2504999999999999</v>
       </c>
-      <c r="N5" s="10"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="6">
         <f>ROUND(M5/M3,4)-1</f>
         <v>0.19140000000000001</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="10">
         <v>1.2482</v>
       </c>
-      <c r="Q5" s="10"/>
+      <c r="Q5" s="11"/>
       <c r="R5" s="6">
         <f>ROUND(P5/P3,4)-1</f>
         <v>0.19179999999999997</v>
@@ -11126,23 +11126,23 @@
       <c r="J6" s="3">
         <v>1.4819</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="12">
         <f>ROUND(J6/J3,4)-1</f>
         <v>0.41199999999999992</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="8">
+      <c r="L6" s="13"/>
+      <c r="M6" s="10">
         <v>1.5116000000000001</v>
       </c>
-      <c r="N6" s="10"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="6">
         <f>ROUND(M6/M3,4)-1</f>
         <v>0.44019999999999992</v>
       </c>
-      <c r="P6" s="8">
+      <c r="P6" s="10">
         <v>1.4991000000000001</v>
       </c>
-      <c r="Q6" s="10"/>
+      <c r="Q6" s="11"/>
       <c r="R6" s="6">
         <f>ROUND(P6/P3,4)-1</f>
         <v>0.43140000000000001</v>
@@ -11162,22 +11162,22 @@
       <c r="J11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="18" t="s">
+      <c r="L11" s="9"/>
+      <c r="M11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="8" t="s">
+      <c r="N11" s="9"/>
+      <c r="O11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="8" t="s">
+      <c r="P11" s="11"/>
+      <c r="Q11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="10"/>
+      <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="I12" s="2" t="s">
@@ -11187,32 +11187,32 @@
         <v>15</v>
       </c>
       <c r="K12" s="2">
-        <v>1.2454000000000001</v>
+        <v>1.2381</v>
       </c>
       <c r="L12" s="6">
         <f>ROUND(K12/M3,4)-1</f>
-        <v>0.18650000000000011</v>
+        <v>0.17959999999999998</v>
       </c>
       <c r="M12" s="2">
-        <v>1.2301</v>
+        <v>1.2310000000000001</v>
       </c>
       <c r="N12" s="6">
         <f>ROUND(M12/P3,4)-1</f>
-        <v>0.1745000000000001</v>
+        <v>0.1754</v>
       </c>
       <c r="O12" s="3">
-        <v>1.2406999999999999</v>
+        <v>1.2423</v>
       </c>
       <c r="P12" s="6">
         <f>ROUND(O12/S3,4)-1</f>
-        <v>0.18149999999999999</v>
+        <v>0.18300000000000005</v>
       </c>
       <c r="Q12" s="3">
-        <v>1.2468999999999999</v>
+        <v>1.2519</v>
       </c>
       <c r="R12" s="6">
         <f>ROUND(Q12/U3,4)-1</f>
-        <v>0.18389999999999995</v>
+        <v>0.18870000000000009</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -11433,6 +11433,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="P3:R3"/>
     <mergeCell ref="P4:Q4"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="O11:P11"/>
@@ -11446,18 +11458,6 @@
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="P3:R3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -11502,25 +11502,25 @@
         <v>2</v>
       </c>
       <c r="I1" s="3"/>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="8" t="s">
+      <c r="K1" s="19"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="8" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="8" t="s">
+      <c r="Q1" s="19"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="10"/>
+      <c r="T1" s="11"/>
       <c r="U1" s="3" t="s">
         <v>7</v>
       </c>
@@ -11538,36 +11538,36 @@
       <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="10"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="9"/>
-      <c r="W2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="11"/>
     </row>
     <row r="3" spans="1:23" ht="37.5" x14ac:dyDescent="0.25">
       <c r="I3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="17"/>
       <c r="K3" s="22"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="13"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="16"/>
       <c r="U3" s="5"/>
     </row>
     <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
@@ -11575,19 +11575,19 @@
         <v>10</v>
       </c>
       <c r="J4" s="3"/>
-      <c r="K4" s="16" t="e">
+      <c r="K4" s="12" t="e">
         <f>J4/J3 -1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="10"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="11"/>
       <c r="O4" s="6" t="e">
         <f>M4/M3 -1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="11"/>
       <c r="R4" s="6" t="e">
         <f>ROUND(P4/P3,4) - 1</f>
         <v>#DIV/0!</v>
@@ -11603,19 +11603,19 @@
         <v>11</v>
       </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="16" t="e">
+      <c r="K5" s="12" t="e">
         <f>ROUND(J5/J3,4) - 1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="10"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="11"/>
       <c r="O5" s="6" t="e">
         <f>ROUND(M5/M3,4)-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="11"/>
       <c r="R5" s="6" t="e">
         <f>ROUND(P5/P3,4)-1</f>
         <v>#DIV/0!</v>
@@ -11631,19 +11631,19 @@
         <v>12</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="16" t="e">
+      <c r="K6" s="12" t="e">
         <f>ROUND(J6/J3,4)-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="10"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="11"/>
       <c r="O6" s="6" t="e">
         <f>ROUND(M6/M3,4)-1</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
       <c r="R6" s="6" t="e">
         <f>ROUND(P6/P3,4)-1</f>
         <v>#DIV/0!</v>
@@ -11661,22 +11661,22 @@
       <c r="J11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="18" t="s">
+      <c r="K11" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L11" s="19"/>
-      <c r="M11" s="18" t="s">
+      <c r="L11" s="9"/>
+      <c r="M11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="8" t="s">
+      <c r="N11" s="9"/>
+      <c r="O11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="8" t="s">
+      <c r="P11" s="11"/>
+      <c r="Q11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="R11" s="10"/>
+      <c r="R11" s="11"/>
     </row>
     <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="I12" s="2" t="s">
@@ -11876,6 +11876,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="U2:W2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="P4:Q4"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="O11:P11"/>
@@ -11886,22 +11902,6 @@
     <mergeCell ref="K6:L6"/>
     <mergeCell ref="M6:N6"/>
     <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="U2:W2"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>